<commit_message>
updated what logic to fix token span errors
</commit_message>
<xml_diff>
--- a/when_test_controls.xlsx
+++ b/when_test_controls.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee8d3d5c28cf10e6/Desktop/final_consolidated_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_BA3195B5035FDA0E62355476585DCE3A17C36E83" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FD39527-A6B0-4654-8A52-02722149ABD9}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_BA3195B5035FDA0E62355476585DCE3A17C36E83" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{428E30EA-E9DB-41C6-A7D8-A6BC16374AA1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WHEN Test Controls" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
   <si>
     <t>TEST-1000</t>
   </si>
@@ -67,48 +68,30 @@
     <t>TEST-1003</t>
   </si>
   <si>
-    <t>The Operations Team reconciles the financial reports to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
     <t>TEST-1004</t>
   </si>
   <si>
-    <t>The Compliance Officer reviews the monthly reconciliations to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>TEST-1005</t>
   </si>
   <si>
-    <t>The IT Administrator reviews the access logs before each financial close to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>before each financial close</t>
   </si>
   <si>
     <t>TEST-1006</t>
   </si>
   <si>
-    <t>The IT Administrator reviews the monthly reconciliations to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>Detective</t>
   </si>
   <si>
     <t>TEST-1007</t>
   </si>
   <si>
-    <t>The Operations Team tests the user entitlements to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>TEST-1008</t>
   </si>
   <si>
-    <t>The Risk Management Department reviews the risk assessments periodically to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>Ad Hoc</t>
   </si>
   <si>
@@ -118,15 +101,9 @@
     <t>TEST-1009</t>
   </si>
   <si>
-    <t>The Audit Committee reconciles the user entitlements periodically to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>TEST-1010</t>
   </si>
   <si>
-    <t>The Accounting Manager reviews the financial reports when appropriate to ensure compliance with internal policies.</t>
-  </si>
-  <si>
     <t>when appropriate</t>
   </si>
   <si>
@@ -293,13 +270,130 @@
   </si>
   <si>
     <t>ad-hoc</t>
+  </si>
+  <si>
+    <t>Exceptions are routed to the appropriate team as needed. Access is restricted to authorized users. The system automatically ages receivables monthly.</t>
+  </si>
+  <si>
+    <t>"Access is limited to authorized personnel."</t>
+  </si>
+  <si>
+    <t>"This control is described in the documentation."</t>
+  </si>
+  <si>
+    <t>"Exceptions are addressed as needed."</t>
+  </si>
+  <si>
+    <t>"Review and approve the invoice, then file it in the archive."</t>
+  </si>
+  <si>
+    <t>"To ensure accuracy, management monitors the reports."</t>
+  </si>
+  <si>
+    <t>Fallback span only</t>
+  </si>
+  <si>
+    <t>Token span conversion in special cases</t>
+  </si>
+  <si>
+    <t>No verbs</t>
+  </si>
+  <si>
+    <t>Safe return even with no control verbs</t>
+  </si>
+  <si>
+    <t>Only vague term</t>
+  </si>
+  <si>
+    <t>Does it skip/penalize vague phrasing correctly</t>
+  </si>
+  <si>
+    <t>Index near token limit</t>
+  </si>
+  <si>
+    <r>
+      <t>Very short doc (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>"Reconcile."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) or very long one</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ensures no </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>token.i + 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> errors</t>
+    </r>
+  </si>
+  <si>
+    <t>Multiple actions</t>
+  </si>
+  <si>
+    <t>Detects compound controls</t>
+  </si>
+  <si>
+    <t>Purpose-only sentence</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ensures </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ensure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> isn't misclassified as WHAT</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +405,19 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -348,11 +455,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,6 +488,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,40 +782,40 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -703,12 +827,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -720,10 +844,10 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -743,12 +867,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -757,15 +881,15 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
+      <c r="B6" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -774,15 +898,18 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -793,53 +920,59 @@
       <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -847,16 +980,16 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -867,16 +1000,16 @@
       <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -888,15 +1021,15 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -908,15 +1041,15 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -931,12 +1064,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -945,18 +1078,18 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -965,41 +1098,41 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1008,12 +1141,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1025,32 +1158,32 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1062,18 +1195,18 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
@@ -1082,35 +1215,35 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1122,29 +1255,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
@@ -1156,49 +1289,49 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
@@ -1207,35 +1340,35 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1247,10 +1380,95 @@
         <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350D0F05-1A3D-405C-BA84-69F5554A73E8}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>